<commit_message>
Nota fiscal e caixa do dia 16
</commit_message>
<xml_diff>
--- a/FLUXO DE CAIXA SETEMBRO 2019/16-09-2019_FluxoDeCaixa.xlsx
+++ b/FLUXO DE CAIXA SETEMBRO 2019/16-09-2019_FluxoDeCaixa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raphael_Campos\Documents\GitHub\ConnectFibra\FLUXO DE CAIXA SETEMBRO 2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EB8C8E7-926E-4AE4-A553-6AD0957DF71C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29059096-0372-4C56-BB23-A65E94295896}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9152A456-9720-4D0C-842A-50118CAD28D0}"/>
   </bookViews>
@@ -537,7 +537,7 @@
   <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>